<commit_message>
48. Check whether a String is Palindrome or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush\eclipse-workspace\CodingProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="493">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1497,6 +1497,18 @@
   </si>
   <si>
     <t>Recursive call to reverse method, keep dividing in half till there is only one element (l+r = complete string)</t>
+  </si>
+  <si>
+    <t>Reverse and compare</t>
+  </si>
+  <si>
+    <t>Compare with two pointers</t>
+  </si>
+  <si>
+    <t>Use maps</t>
+  </si>
+  <si>
+    <t>Use array</t>
   </si>
 </sst>
 </file>
@@ -1928,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="98" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2774,6 +2786,12 @@
       <c r="D57" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E57" t="s">
+        <v>489</v>
+      </c>
+      <c r="F57" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="58" spans="1:9" ht="21">
       <c r="A58" s="5" t="s">
@@ -2787,7 +2805,13 @@
         <v>56</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="E58" t="s">
+        <v>491</v>
+      </c>
+      <c r="F58" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="21">

</xml_diff>

<commit_message>
Check whether a String is Palindrome or not .
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1941,7 +1941,7 @@
   <dimension ref="A1:I481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2784,7 +2784,7 @@
         <v>55</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
       <c r="E57" t="s">
         <v>489</v>

</xml_diff>

<commit_message>
7. cyclically rotate an array by one
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="495">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1463,9 +1463,6 @@
     <t>Partition process of quick sort (partition at 0- swap if number is less, to the beginning location)</t>
   </si>
   <si>
-    <t>Two pointers. If left right both negative, increase. Else swap</t>
-  </si>
-  <si>
     <t>Can apply sort</t>
   </si>
   <si>
@@ -1509,6 +1506,15 @@
   </si>
   <si>
     <t>Use array</t>
+  </si>
+  <si>
+    <t>Two pointers. If left right both negative, left++, if both negative right++. Else swap</t>
+  </si>
+  <si>
+    <t>Save last element in a temp variable, shift positions</t>
+  </si>
+  <si>
+    <t>Can make a new array</t>
   </si>
 </sst>
 </file>
@@ -1940,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="98" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1949,7 +1955,7 @@
     <col min="1" max="1" width="13.19921875" customWidth="1"/>
     <col min="2" max="2" width="8.3984375" customWidth="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="8.296875" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
     <col min="7" max="7" width="34.296875" customWidth="1"/>
   </cols>
@@ -1969,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -1979,9 +1985,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="21">
       <c r="A6" s="5" t="s">
@@ -2090,10 +2094,10 @@
         <v>476</v>
       </c>
       <c r="G10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H10" t="s">
-        <v>477</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21">
@@ -2123,7 +2127,13 @@
         <v>12</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="E12" t="s">
+        <v>493</v>
+      </c>
+      <c r="F12" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21">
@@ -2186,16 +2196,16 @@
         <v>465</v>
       </c>
       <c r="E16" t="s">
+        <v>479</v>
+      </c>
+      <c r="F16" t="s">
         <v>480</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>481</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>482</v>
-      </c>
-      <c r="H16" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21">
@@ -2757,19 +2767,19 @@
         <v>465</v>
       </c>
       <c r="E56" t="s">
+        <v>483</v>
+      </c>
+      <c r="F56" t="s">
         <v>484</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>485</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>486</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>487</v>
-      </c>
-      <c r="I56" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="21">
@@ -2787,10 +2797,10 @@
         <v>465</v>
       </c>
       <c r="E57" t="s">
+        <v>488</v>
+      </c>
+      <c r="F57" t="s">
         <v>489</v>
-      </c>
-      <c r="F57" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="21">
@@ -2808,10 +2818,10 @@
         <v>465</v>
       </c>
       <c r="E58" t="s">
+        <v>490</v>
+      </c>
+      <c r="F58" t="s">
         <v>491</v>
-      </c>
-      <c r="F58" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="21">

</xml_diff>

<commit_message>
10. Minimum no. of Jumps to reach end of an array (recursive)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush\eclipse-workspace\CodingProblems\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10908" windowHeight="3840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="503">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1524,13 +1520,28 @@
   </si>
   <si>
     <t>in c++ array variable points to the first element</t>
+  </si>
+  <si>
+    <t>Swap shorter from second array, sort both arrays</t>
+  </si>
+  <si>
+    <t>Join Both Array and try to sort.</t>
+  </si>
+  <si>
+    <t>Used shell sort</t>
+  </si>
+  <si>
+    <t>Recursive (take one jump, call method again, if length reached, reutrn 1)</t>
+  </si>
+  <si>
+    <t>Try DP approach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1592,6 +1603,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Urw-din"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1614,7 +1630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,6 +1654,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1955,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2198,6 +2215,12 @@
       <c r="D15" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E15" t="s">
+        <v>501</v>
+      </c>
+      <c r="F15" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="21">
       <c r="A16" s="5" t="s">
@@ -2226,7 +2249,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="21">
+    <row r="17" spans="1:7" ht="21">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2240,8 +2263,17 @@
       <c r="D17" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="21">
+      <c r="E17" t="s">
+        <v>498</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="G17" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2256,7 +2288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21">
+    <row r="19" spans="1:7" ht="21">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2271,7 +2303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="21">
+    <row r="20" spans="1:7" ht="21">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2286,7 +2318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21">
+    <row r="21" spans="1:7" ht="21">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2301,7 +2333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="21">
+    <row r="22" spans="1:7" ht="21">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2316,7 +2348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21">
+    <row r="23" spans="1:7" ht="21">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2331,7 +2363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="21">
+    <row r="24" spans="1:7" ht="21">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2346,7 +2378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="21">
+    <row r="25" spans="1:7" ht="21">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2361,7 +2393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="21">
+    <row r="26" spans="1:7" ht="21">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2376,7 +2408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21">
+    <row r="27" spans="1:7" ht="21">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2391,7 +2423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21">
+    <row r="28" spans="1:7" ht="21">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -2406,7 +2438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="21">
+    <row r="29" spans="1:7" ht="21">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -2421,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21">
+    <row r="30" spans="1:7" ht="21">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -2436,7 +2468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="21">
+    <row r="31" spans="1:7" ht="21">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
@@ -2451,7 +2483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="21">
+    <row r="32" spans="1:7" ht="21">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
22. Find factorial of a large number
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush\eclipse-workspace\CodingProblems\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10908" windowHeight="3840"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="509">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1535,6 +1539,24 @@
   </si>
   <si>
     <t>Try DP approach</t>
+  </si>
+  <si>
+    <t>If you can take 4 steps doesn't mean you must take 4 steps, take the max step</t>
+  </si>
+  <si>
+    <t>Greedy approach</t>
+  </si>
+  <si>
+    <t>What if multiple same numbers? Choose the farthest</t>
+  </si>
+  <si>
+    <t>Find common between two. Then the third</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Recursion</t>
   </si>
 </sst>
 </file>
@@ -1972,8 +1994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1986,17 +2008,17 @@
     <col min="7" max="7" width="34.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.6">
+    <row r="1" spans="1:9" ht="24.6">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="C2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21">
+    <row r="4" spans="1:9" ht="21">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2010,10 +2032,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="21">
+    <row r="6" spans="1:9" ht="21">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -2033,7 +2055,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21">
+    <row r="7" spans="1:9" ht="21">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2054,7 +2076,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21">
+    <row r="8" spans="1:9" ht="21">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -2075,7 +2097,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21">
+    <row r="9" spans="1:9" ht="21">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -2099,7 +2121,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21">
+    <row r="10" spans="1:9" ht="21">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -2126,7 +2148,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21">
+    <row r="11" spans="1:9" ht="21">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -2150,7 +2172,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="21">
+    <row r="12" spans="1:9" ht="21">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2193,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21">
+    <row r="13" spans="1:9" ht="21">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2186,7 +2208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="21">
+    <row r="14" spans="1:9" ht="21">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -2201,7 +2223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21">
+    <row r="15" spans="1:9" ht="21">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2221,8 +2243,17 @@
       <c r="F15" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="21">
+      <c r="G15" t="s">
+        <v>503</v>
+      </c>
+      <c r="H15" t="s">
+        <v>504</v>
+      </c>
+      <c r="I15" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2377,6 +2408,9 @@
       <c r="D24" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E24" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="21">
       <c r="A25" s="5" t="s">
@@ -2421,6 +2455,12 @@
       </c>
       <c r="D27" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>507</v>
+      </c>
+      <c r="F27" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="21">
@@ -2797,6 +2837,7 @@
         <v>4</v>
       </c>
     </row>
+    <row r="54" spans="1:9" ht="23.4" customHeight="1"/>
     <row r="55" spans="1:9" ht="21">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>

</xml_diff>

<commit_message>
51. Check whether one string is a rotation of another
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="510">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1553,10 +1553,13 @@
     <t>Find common between two. Then the third</t>
   </si>
   <si>
-    <t>DP</t>
-  </si>
-  <si>
-    <t>Recursion</t>
+    <t>DP-with BigInt</t>
+  </si>
+  <si>
+    <t>if a+a contains b, also lengths should be same</t>
+  </si>
+  <si>
+    <t>Push a and b in queues. Pop and push b's element for one length (Queue=new linkedlist), if you use DEQUEUE, then order gets reversed</t>
   </si>
 </sst>
 </file>
@@ -1994,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="88" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2459,9 +2462,6 @@
       <c r="E27" t="s">
         <v>507</v>
       </c>
-      <c r="F27" t="s">
-        <v>508</v>
-      </c>
     </row>
     <row r="28" spans="1:7" ht="21">
       <c r="A28" s="5" t="s">
@@ -2942,7 +2942,13 @@
         <v>58</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="E60" t="s">
+        <v>508</v>
+      </c>
+      <c r="F60" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="21">

</xml_diff>

<commit_message>
52. Check whether a string is a valid shuffle of two strings or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="513">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1560,6 +1560,15 @@
   </si>
   <si>
     <t>Push a and b in queues. Pop and push b's element for one length (Queue=new linkedlist), if you use DEQUEUE, then order gets reversed</t>
+  </si>
+  <si>
+    <t>Sort the arrays and return</t>
+  </si>
+  <si>
+    <t>Can put in Tree map and compare</t>
+  </si>
+  <si>
+    <t>Use Arrays.equals</t>
   </si>
 </sst>
 </file>
@@ -1997,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="88" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="B53" zoomScale="88" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2963,7 +2972,16 @@
         <v>59</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="E61" t="s">
+        <v>511</v>
+      </c>
+      <c r="F61" t="s">
+        <v>510</v>
+      </c>
+      <c r="G61" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="21">

</xml_diff>

<commit_message>
75. Find the first repeated word in string.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="514">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1569,6 +1569,9 @@
   </si>
   <si>
     <t>Use Arrays.equals</t>
+  </si>
+  <si>
+    <t>Make a list of values, fetch key for that value</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" zoomScale="88" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3269,7 +3272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="21">
+    <row r="81" spans="1:5" ht="21">
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
@@ -3284,7 +3287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="21">
+    <row r="82" spans="1:5" ht="21">
       <c r="A82" s="5" t="s">
         <v>53</v>
       </c>
@@ -3299,7 +3302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="21">
+    <row r="83" spans="1:5" ht="21">
       <c r="A83" s="5" t="s">
         <v>53</v>
       </c>
@@ -3314,7 +3317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="21">
+    <row r="84" spans="1:5" ht="21">
       <c r="A84" s="5" t="s">
         <v>53</v>
       </c>
@@ -3328,8 +3331,11 @@
       <c r="D84" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="21">
+      <c r="E84" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="21">
       <c r="A85" s="5" t="s">
         <v>53</v>
       </c>
@@ -3344,7 +3350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="21">
+    <row r="86" spans="1:5" ht="21">
       <c r="A86" s="5" t="s">
         <v>53</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="21">
+    <row r="87" spans="1:5" ht="21">
       <c r="A87" s="5" t="s">
         <v>53</v>
       </c>
@@ -3374,7 +3380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="21">
+    <row r="88" spans="1:5" ht="21">
       <c r="A88" s="5" t="s">
         <v>53</v>
       </c>
@@ -3389,7 +3395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="21">
+    <row r="89" spans="1:5" ht="21">
       <c r="A89" s="5" t="s">
         <v>53</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="21">
+    <row r="90" spans="1:5" ht="21">
       <c r="A90" s="5" t="s">
         <v>53</v>
       </c>
@@ -3419,7 +3425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="21">
+    <row r="91" spans="1:5" ht="21">
       <c r="A91" s="5" t="s">
         <v>53</v>
       </c>
@@ -3434,7 +3440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="21">
+    <row r="92" spans="1:5" ht="21">
       <c r="A92" s="5" t="s">
         <v>53</v>
       </c>
@@ -3449,7 +3455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="21">
+    <row r="93" spans="1:5" ht="21">
       <c r="A93" s="5" t="s">
         <v>53</v>
       </c>
@@ -3464,7 +3470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="21">
+    <row r="94" spans="1:5" ht="21">
       <c r="A94" s="5" t="s">
         <v>53</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="21">
+    <row r="95" spans="1:5" ht="21">
       <c r="A95" s="5" t="s">
         <v>53</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="21">
+    <row r="96" spans="1:5" ht="21">
       <c r="A96" s="5" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
67. Minimum number of bracket reversals needed to make an expression balanced.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="517">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1572,6 +1572,15 @@
   </si>
   <si>
     <t>Make a list of values, fetch key for that value</t>
+  </si>
+  <si>
+    <t>Pop balanced brackets, remaining ceil(close/2)+ceil(open/2), they should be double</t>
+  </si>
+  <si>
+    <t>Count with 2 vars left and right, increase left if found. Decrease it if right found else increase right</t>
+  </si>
+  <si>
+    <t>One pointer in similar way</t>
   </si>
 </sst>
 </file>
@@ -2009,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="B60" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3032,7 +3041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="21">
+    <row r="65" spans="1:7" ht="21">
       <c r="A65" s="5" t="s">
         <v>53</v>
       </c>
@@ -3047,7 +3056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="21">
+    <row r="66" spans="1:7" ht="21">
       <c r="A66" s="5" t="s">
         <v>53</v>
       </c>
@@ -3062,7 +3071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="21">
+    <row r="67" spans="1:7" ht="21">
       <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
@@ -3077,7 +3086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="21">
+    <row r="68" spans="1:7" ht="21">
       <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
@@ -3092,7 +3101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="21">
+    <row r="69" spans="1:7" ht="21">
       <c r="A69" s="5" t="s">
         <v>53</v>
       </c>
@@ -3107,7 +3116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="21">
+    <row r="70" spans="1:7" ht="21">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
@@ -3122,7 +3131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="21">
+    <row r="71" spans="1:7" ht="21">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -3137,7 +3146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="21">
+    <row r="72" spans="1:7" ht="21">
       <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
@@ -3152,7 +3161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="21">
+    <row r="73" spans="1:7" ht="21">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="21">
+    <row r="74" spans="1:7" ht="21">
       <c r="A74" s="5" t="s">
         <v>53</v>
       </c>
@@ -3182,7 +3191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="21">
+    <row r="75" spans="1:7" ht="21">
       <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
@@ -3197,7 +3206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="21">
+    <row r="76" spans="1:7" ht="21">
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
@@ -3209,10 +3218,19 @@
         <v>74</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="21">
+        <v>465</v>
+      </c>
+      <c r="E76" t="s">
+        <v>514</v>
+      </c>
+      <c r="F76" t="s">
+        <v>515</v>
+      </c>
+      <c r="G76" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="21">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -3227,7 +3245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="21">
+    <row r="78" spans="1:7" ht="21">
       <c r="A78" s="5" t="s">
         <v>53</v>
       </c>
@@ -3242,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="21">
+    <row r="79" spans="1:7" ht="21">
       <c r="A79" s="5" t="s">
         <v>53</v>
       </c>
@@ -3257,7 +3275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="21">
+    <row r="80" spans="1:7" ht="21">
       <c r="A80" s="5" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
9. Maximize the heights and minimize the difference between the extremes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="528">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1608,6 +1608,12 @@
   </si>
   <si>
     <t>max_so_far=a[0], curr_max=a[0];  curr_max=Math.max(a[i],curr_max+a[i]);  max_so_far=Math.max(curr_max,max_so_far);</t>
+  </si>
+  <si>
+    <t>Same Kadane's algorightm</t>
+  </si>
+  <si>
+    <t>Sort, increase left side, decrease right side. Needs more refinement</t>
   </si>
 </sst>
 </file>
@@ -2052,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2265,6 +2271,9 @@
       <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E13" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="21">
       <c r="A14" s="5" t="s">
@@ -2279,6 +2288,9 @@
       </c>
       <c r="D14" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="21">

</xml_diff>

<commit_message>
62. Balanced Parenthesis problem
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="533">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1617,6 +1617,18 @@
   </si>
   <si>
     <t>Basic - try n^2</t>
+  </si>
+  <si>
+    <t>Store in map with frequency. If the number is half of the sum, then count to make all n! times {1,1,1,1) (2), if not count half of the times complementary is found in map</t>
+  </si>
+  <si>
+    <t>Kepp pointer to track negative number, swap.</t>
+  </si>
+  <si>
+    <t>Contd</t>
+  </si>
+  <si>
+    <t>Stacks</t>
   </si>
 </sst>
 </file>
@@ -2061,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="88" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2496,6 +2508,9 @@
       <c r="E23" t="s">
         <v>528</v>
       </c>
+      <c r="F23" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="21">
       <c r="A24" s="5" t="s">
@@ -2529,6 +2544,9 @@
       <c r="D25" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E25" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="21">
       <c r="A26" s="5" t="s">
@@ -2544,6 +2562,9 @@
       <c r="D26" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E26" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="21">
       <c r="A27" s="5" t="s">
@@ -2576,6 +2597,9 @@
       </c>
       <c r="D28" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="21">
@@ -3222,7 +3246,10 @@
         <v>69</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="E71" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="21">

</xml_diff>

<commit_message>
96. Find the repeating and the missing
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="543">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1638,13 +1638,34 @@
   </si>
   <si>
     <t>if (a[i] == i + 1)</t>
+  </si>
+  <si>
+    <t>Middle of 3 elements</t>
+  </si>
+  <si>
+    <t>map[a[i]-1]++, check if value is zero or two.</t>
+  </si>
+  <si>
+    <t>Same with map</t>
+  </si>
+  <si>
+    <t>Sort and traverse for repeated and missing element</t>
+  </si>
+  <si>
+    <t>Make two equations S = n(n+1)/2 - x + y P = 1*2*3*...*n * y / x Solve for x and y</t>
+  </si>
+  <si>
+    <t>Make two equations using sum and sum of squares</t>
+  </si>
+  <si>
+    <t>Using OR Operator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1717,6 +1738,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1739,7 +1768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1765,6 +1794,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2080,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I481"/>
+  <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="88" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="D96" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K101" sqref="K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3651,7 +3681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="21">
+    <row r="97" spans="1:10" ht="21">
       <c r="A97" s="5" t="s">
         <v>53</v>
       </c>
@@ -3666,7 +3696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="21">
+    <row r="98" spans="1:10" ht="21">
       <c r="A98" s="5" t="s">
         <v>53</v>
       </c>
@@ -3681,13 +3711,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="21">
+    <row r="100" spans="1:10" ht="21">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="7"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:5" ht="21">
+    <row r="101" spans="1:10" ht="21">
       <c r="A101" s="5" t="s">
         <v>97</v>
       </c>
@@ -3705,7 +3735,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="21">
+    <row r="102" spans="1:10" ht="21">
       <c r="A102" s="5" t="s">
         <v>97</v>
       </c>
@@ -3723,7 +3753,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="21">
+    <row r="103" spans="1:10" ht="21">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -3738,7 +3768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="21">
+    <row r="104" spans="1:10" ht="21">
       <c r="A104" s="5" t="s">
         <v>97</v>
       </c>
@@ -3756,7 +3786,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="21">
+    <row r="105" spans="1:10" ht="21">
       <c r="A105" s="5" t="s">
         <v>97</v>
       </c>
@@ -3768,10 +3798,13 @@
         <v>102</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="21">
+        <v>465</v>
+      </c>
+      <c r="E105" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="21">
       <c r="A106" s="5" t="s">
         <v>97</v>
       </c>
@@ -3786,7 +3819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="21">
+    <row r="107" spans="1:10" ht="21">
       <c r="A107" s="5" t="s">
         <v>97</v>
       </c>
@@ -3798,10 +3831,28 @@
         <v>104</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="21">
+        <v>531</v>
+      </c>
+      <c r="E107" t="s">
+        <v>537</v>
+      </c>
+      <c r="F107" t="s">
+        <v>538</v>
+      </c>
+      <c r="G107" t="s">
+        <v>539</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>540</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="J107" s="13" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="21">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
@@ -3816,7 +3867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="21">
+    <row r="109" spans="1:10" ht="21">
       <c r="A109" s="5" t="s">
         <v>97</v>
       </c>
@@ -3831,7 +3882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="21">
+    <row r="110" spans="1:10" ht="21">
       <c r="A110" s="5" t="s">
         <v>97</v>
       </c>
@@ -3846,7 +3897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="21">
+    <row r="111" spans="1:10" ht="21">
       <c r="A111" s="5" t="s">
         <v>97</v>
       </c>
@@ -3861,7 +3912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="21">
+    <row r="112" spans="1:10" ht="21">
       <c r="A112" s="5" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
Updates in Excel and gitignore
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="548">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1659,13 +1659,28 @@
   </si>
   <si>
     <t>Using OR Operator</t>
+  </si>
+  <si>
+    <t>Count in map</t>
+  </si>
+  <si>
+    <t>Track till n/2 in 2 nested for loops for each number</t>
+  </si>
+  <si>
+    <t>Using BST</t>
+  </si>
+  <si>
+    <t>Moore’s Voting Algorithm</t>
+  </si>
+  <si>
+    <t>sort the array, update the count until the present element is similar to the previous one</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1746,6 +1761,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1768,7 +1789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1795,6 +1816,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2112,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D96" zoomScale="88" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3864,7 +3886,22 @@
         <v>105</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>4</v>
+        <v>531</v>
+      </c>
+      <c r="E108" t="s">
+        <v>543</v>
+      </c>
+      <c r="F108" t="s">
+        <v>544</v>
+      </c>
+      <c r="G108" t="s">
+        <v>545</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>546</v>
+      </c>
+      <c r="I108" s="14" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="21">

</xml_diff>

<commit_message>
25. Find all elements that appear more than " n/k " times.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -2134,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5411,7 +5411,9 @@
       <c r="A214" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="5"/>
+      <c r="B214" s="5">
+        <v>197</v>
+      </c>
       <c r="C214" s="6" t="s">
         <v>208</v>
       </c>
@@ -5423,7 +5425,9 @@
       <c r="A215" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B215" s="5"/>
+      <c r="B215" s="5">
+        <v>198</v>
+      </c>
       <c r="C215" s="6" t="s">
         <v>209</v>
       </c>
@@ -5435,7 +5439,9 @@
       <c r="A216" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B216" s="5"/>
+      <c r="B216" s="5">
+        <v>199</v>
+      </c>
       <c r="C216" s="6" t="s">
         <v>210</v>
       </c>
@@ -5447,7 +5453,9 @@
       <c r="A217" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B217" s="5"/>
+      <c r="B217" s="5">
+        <v>200</v>
+      </c>
       <c r="C217" s="6" t="s">
         <v>211</v>
       </c>
@@ -5459,7 +5467,9 @@
       <c r="A218" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B218" s="5"/>
+      <c r="B218" s="5">
+        <v>201</v>
+      </c>
       <c r="C218" s="6" t="s">
         <v>212</v>
       </c>
@@ -5471,7 +5481,9 @@
       <c r="A219" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B219" s="5"/>
+      <c r="B219" s="5">
+        <v>202</v>
+      </c>
       <c r="C219" s="6" t="s">
         <v>213</v>
       </c>
@@ -5483,7 +5495,9 @@
       <c r="A220" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B220" s="5"/>
+      <c r="B220" s="5">
+        <v>203</v>
+      </c>
       <c r="C220" s="9" t="s">
         <v>214</v>
       </c>
@@ -5495,7 +5509,9 @@
       <c r="A221" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B221" s="5"/>
+      <c r="B221" s="5">
+        <v>204</v>
+      </c>
       <c r="C221" s="6" t="s">
         <v>215</v>
       </c>
@@ -5507,7 +5523,9 @@
       <c r="A222" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B222" s="5"/>
+      <c r="B222" s="5">
+        <v>205</v>
+      </c>
       <c r="C222" s="6" t="s">
         <v>216</v>
       </c>
@@ -5519,7 +5537,9 @@
       <c r="A223" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B223" s="5"/>
+      <c r="B223" s="5">
+        <v>206</v>
+      </c>
       <c r="C223" s="6" t="s">
         <v>217</v>
       </c>
@@ -5531,7 +5551,9 @@
       <c r="A224" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B224" s="5"/>
+      <c r="B224" s="5">
+        <v>207</v>
+      </c>
       <c r="C224" s="6" t="s">
         <v>218</v>
       </c>
@@ -5543,7 +5565,9 @@
       <c r="A225" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B225" s="5"/>
+      <c r="B225" s="5">
+        <v>208</v>
+      </c>
       <c r="C225" s="6" t="s">
         <v>219</v>
       </c>
@@ -5555,7 +5579,9 @@
       <c r="A226" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B226" s="5"/>
+      <c r="B226" s="5">
+        <v>209</v>
+      </c>
       <c r="C226" s="6" t="s">
         <v>220</v>
       </c>
@@ -5567,7 +5593,9 @@
       <c r="A227" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B227" s="5"/>
+      <c r="B227" s="5">
+        <v>210</v>
+      </c>
       <c r="C227" s="6" t="s">
         <v>221</v>
       </c>
@@ -5579,7 +5607,9 @@
       <c r="A228" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B228" s="5"/>
+      <c r="B228" s="5">
+        <v>211</v>
+      </c>
       <c r="C228" s="6" t="s">
         <v>222</v>
       </c>
@@ -5591,7 +5621,9 @@
       <c r="A229" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B229" s="5"/>
+      <c r="B229" s="5">
+        <v>212</v>
+      </c>
       <c r="C229" s="6" t="s">
         <v>223</v>
       </c>
@@ -5603,7 +5635,9 @@
       <c r="A230" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B230" s="5"/>
+      <c r="B230" s="5">
+        <v>213</v>
+      </c>
       <c r="C230" s="6" t="s">
         <v>224</v>
       </c>
@@ -5615,7 +5649,9 @@
       <c r="A231" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B231" s="5"/>
+      <c r="B231" s="5">
+        <v>214</v>
+      </c>
       <c r="C231" s="6" t="s">
         <v>225</v>
       </c>
@@ -5627,7 +5663,9 @@
       <c r="A232" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B232" s="5"/>
+      <c r="B232" s="5">
+        <v>215</v>
+      </c>
       <c r="C232" s="6" t="s">
         <v>226</v>
       </c>
@@ -5639,7 +5677,9 @@
       <c r="A233" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B233" s="5"/>
+      <c r="B233" s="5">
+        <v>216</v>
+      </c>
       <c r="C233" s="6" t="s">
         <v>227</v>
       </c>
@@ -5651,7 +5691,9 @@
       <c r="A234" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B234" s="5"/>
+      <c r="B234" s="5">
+        <v>217</v>
+      </c>
       <c r="C234" s="6" t="s">
         <v>228</v>
       </c>
@@ -5663,7 +5705,9 @@
       <c r="A235" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B235" s="5"/>
+      <c r="B235" s="5">
+        <v>218</v>
+      </c>
       <c r="C235" s="6" t="s">
         <v>229</v>
       </c>
@@ -5683,7 +5727,9 @@
       <c r="A238" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B238" s="5"/>
+      <c r="B238" s="5">
+        <v>219</v>
+      </c>
       <c r="C238" s="6" t="s">
         <v>231</v>
       </c>
@@ -5695,7 +5741,9 @@
       <c r="A239" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B239" s="5"/>
+      <c r="B239" s="5">
+        <v>220</v>
+      </c>
       <c r="C239" s="6" t="s">
         <v>232</v>
       </c>
@@ -5707,7 +5755,9 @@
       <c r="A240" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B240" s="5"/>
+      <c r="B240" s="5">
+        <v>221</v>
+      </c>
       <c r="C240" s="6" t="s">
         <v>233</v>
       </c>
@@ -5719,7 +5769,9 @@
       <c r="A241" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B241" s="5"/>
+      <c r="B241" s="5">
+        <v>222</v>
+      </c>
       <c r="C241" s="6" t="s">
         <v>234</v>
       </c>
@@ -5731,7 +5783,9 @@
       <c r="A242" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B242" s="5"/>
+      <c r="B242" s="5">
+        <v>223</v>
+      </c>
       <c r="C242" s="6" t="s">
         <v>235</v>
       </c>
@@ -5743,7 +5797,9 @@
       <c r="A243" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B243" s="5"/>
+      <c r="B243" s="5">
+        <v>224</v>
+      </c>
       <c r="C243" s="6" t="s">
         <v>236</v>
       </c>
@@ -5755,7 +5811,9 @@
       <c r="A244" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B244" s="5"/>
+      <c r="B244" s="5">
+        <v>225</v>
+      </c>
       <c r="C244" s="6" t="s">
         <v>237</v>
       </c>
@@ -5767,7 +5825,9 @@
       <c r="A245" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B245" s="5"/>
+      <c r="B245" s="5">
+        <v>226</v>
+      </c>
       <c r="C245" s="6" t="s">
         <v>238</v>
       </c>
@@ -5779,7 +5839,9 @@
       <c r="A246" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B246" s="5"/>
+      <c r="B246" s="5">
+        <v>227</v>
+      </c>
       <c r="C246" s="6" t="s">
         <v>239</v>
       </c>
@@ -5791,7 +5853,9 @@
       <c r="A247" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B247" s="5"/>
+      <c r="B247" s="5">
+        <v>228</v>
+      </c>
       <c r="C247" s="6" t="s">
         <v>240</v>
       </c>
@@ -5803,7 +5867,9 @@
       <c r="A248" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B248" s="5"/>
+      <c r="B248" s="5">
+        <v>229</v>
+      </c>
       <c r="C248" s="6" t="s">
         <v>241</v>
       </c>
@@ -5815,7 +5881,9 @@
       <c r="A249" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B249" s="5"/>
+      <c r="B249" s="5">
+        <v>230</v>
+      </c>
       <c r="C249" s="6" t="s">
         <v>242</v>
       </c>
@@ -5827,7 +5895,9 @@
       <c r="A250" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B250" s="5"/>
+      <c r="B250" s="5">
+        <v>231</v>
+      </c>
       <c r="C250" s="6" t="s">
         <v>243</v>
       </c>
@@ -5839,7 +5909,9 @@
       <c r="A251" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B251" s="5"/>
+      <c r="B251" s="5">
+        <v>232</v>
+      </c>
       <c r="C251" s="6" t="s">
         <v>244</v>
       </c>
@@ -5851,7 +5923,9 @@
       <c r="A252" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B252" s="5"/>
+      <c r="B252" s="5">
+        <v>233</v>
+      </c>
       <c r="C252" s="6" t="s">
         <v>245</v>
       </c>
@@ -5863,7 +5937,9 @@
       <c r="A253" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B253" s="5"/>
+      <c r="B253" s="5">
+        <v>234</v>
+      </c>
       <c r="C253" s="6" t="s">
         <v>246</v>
       </c>
@@ -5875,7 +5951,9 @@
       <c r="A254" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B254" s="5"/>
+      <c r="B254" s="5">
+        <v>235</v>
+      </c>
       <c r="C254" s="6" t="s">
         <v>247</v>
       </c>
@@ -5887,7 +5965,9 @@
       <c r="A255" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B255" s="5"/>
+      <c r="B255" s="5">
+        <v>236</v>
+      </c>
       <c r="C255" s="6" t="s">
         <v>248</v>
       </c>
@@ -5899,7 +5979,9 @@
       <c r="A256" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B256" s="5"/>
+      <c r="B256" s="5">
+        <v>237</v>
+      </c>
       <c r="C256" s="6" t="s">
         <v>249</v>
       </c>
@@ -5911,7 +5993,9 @@
       <c r="A257" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B257" s="5"/>
+      <c r="B257" s="5">
+        <v>238</v>
+      </c>
       <c r="C257" s="6" t="s">
         <v>250</v>
       </c>
@@ -5923,7 +6007,9 @@
       <c r="A258" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B258" s="5"/>
+      <c r="B258" s="5">
+        <v>239</v>
+      </c>
       <c r="C258" s="6" t="s">
         <v>251</v>
       </c>
@@ -5935,7 +6021,9 @@
       <c r="A259" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B259" s="5"/>
+      <c r="B259" s="5">
+        <v>240</v>
+      </c>
       <c r="C259" s="6" t="s">
         <v>252</v>
       </c>
@@ -5947,7 +6035,9 @@
       <c r="A260" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B260" s="5"/>
+      <c r="B260" s="5">
+        <v>241</v>
+      </c>
       <c r="C260" s="6" t="s">
         <v>253</v>
       </c>
@@ -5959,7 +6049,9 @@
       <c r="A261" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B261" s="5"/>
+      <c r="B261" s="5">
+        <v>242</v>
+      </c>
       <c r="C261" s="6" t="s">
         <v>254</v>
       </c>
@@ -5971,7 +6063,9 @@
       <c r="A262" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B262" s="5"/>
+      <c r="B262" s="5">
+        <v>243</v>
+      </c>
       <c r="C262" s="6" t="s">
         <v>255</v>
       </c>
@@ -5983,7 +6077,9 @@
       <c r="A263" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B263" s="5"/>
+      <c r="B263" s="5">
+        <v>244</v>
+      </c>
       <c r="C263" s="6" t="s">
         <v>256</v>
       </c>
@@ -5995,7 +6091,9 @@
       <c r="A264" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B264" s="5"/>
+      <c r="B264" s="5">
+        <v>245</v>
+      </c>
       <c r="C264" s="6" t="s">
         <v>257</v>
       </c>
@@ -6007,7 +6105,9 @@
       <c r="A265" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B265" s="5"/>
+      <c r="B265" s="5">
+        <v>246</v>
+      </c>
       <c r="C265" s="6" t="s">
         <v>258</v>
       </c>
@@ -6019,7 +6119,9 @@
       <c r="A266" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B266" s="5"/>
+      <c r="B266" s="5">
+        <v>247</v>
+      </c>
       <c r="C266" s="6" t="s">
         <v>259</v>
       </c>
@@ -6031,7 +6133,9 @@
       <c r="A267" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B267" s="5"/>
+      <c r="B267" s="5">
+        <v>248</v>
+      </c>
       <c r="C267" s="6" t="s">
         <v>260</v>
       </c>
@@ -6043,7 +6147,9 @@
       <c r="A268" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B268" s="5"/>
+      <c r="B268" s="5">
+        <v>249</v>
+      </c>
       <c r="C268" s="6" t="s">
         <v>261</v>
       </c>
@@ -6055,7 +6161,9 @@
       <c r="A269" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B269" s="5"/>
+      <c r="B269" s="5">
+        <v>250</v>
+      </c>
       <c r="C269" s="6" t="s">
         <v>262</v>
       </c>
@@ -6067,7 +6175,9 @@
       <c r="A270" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B270" s="5"/>
+      <c r="B270" s="5">
+        <v>251</v>
+      </c>
       <c r="C270" s="6" t="s">
         <v>263</v>
       </c>
@@ -6079,7 +6189,9 @@
       <c r="A271" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B271" s="5"/>
+      <c r="B271" s="5">
+        <v>252</v>
+      </c>
       <c r="C271" s="6" t="s">
         <v>87</v>
       </c>
@@ -6091,7 +6203,9 @@
       <c r="A272" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B272" s="5"/>
+      <c r="B272" s="5">
+        <v>253</v>
+      </c>
       <c r="C272" s="6" t="s">
         <v>264</v>
       </c>

</xml_diff>

<commit_message>
Committing Work in Progress files
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="554">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1674,13 +1674,31 @@
   </si>
   <si>
     <t>sort the array, update the count until the present element is similar to the previous one</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>If odd= a[n/2] else 0.5*a[n/2]+a[n/2-1]</t>
+  </si>
+  <si>
+    <t>median will be average of elements at index n-1 and n in the array obtained after merging ar1 and ar2</t>
+  </si>
+  <si>
+    <t>median will be average of elements at index ((m+n)/2 - 1) and (m+n)/2 in the array obtained after merging ar1 and ar2</t>
+  </si>
+  <si>
+    <t>Put in map. Check count</t>
+  </si>
+  <si>
+    <t>Can put the count in an a[10000] array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1767,6 +1785,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF75715E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1789,7 +1819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1817,6 +1847,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2134,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C273" sqref="C273"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2690,7 +2726,10 @@
         <v>30</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="E30" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="21">
@@ -2720,10 +2759,16 @@
         <v>32</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="21">
+        <v>465</v>
+      </c>
+      <c r="E32" t="s">
+        <v>552</v>
+      </c>
+      <c r="F32" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="21">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -2738,7 +2783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21">
+    <row r="34" spans="1:6" ht="21">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2753,7 +2798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="21">
+    <row r="35" spans="1:6" ht="21">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
@@ -2768,7 +2813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="21">
+    <row r="36" spans="1:6" ht="21">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -2783,7 +2828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21">
+    <row r="37" spans="1:6" ht="21">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
@@ -2798,7 +2843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21">
+    <row r="38" spans="1:6" ht="21">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -2813,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="21">
+    <row r="39" spans="1:6" ht="21">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -2828,7 +2873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="21">
+    <row r="40" spans="1:6" ht="21">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -2840,10 +2885,16 @@
         <v>40</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="21">
+        <v>465</v>
+      </c>
+      <c r="E40" t="s">
+        <v>549</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="21">
       <c r="A41" s="5" t="s">
         <v>5</v>
       </c>
@@ -2855,24 +2906,30 @@
         <v>41</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="21">
+        <v>531</v>
+      </c>
+      <c r="E41" t="s">
+        <v>551</v>
+      </c>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="1:6" ht="21">
       <c r="C42" s="7"/>
       <c r="D42" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="21">
+      <c r="F42" s="16"/>
+    </row>
+    <row r="43" spans="1:6" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="7"/>
       <c r="D43" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="21">
+      <c r="F43" s="16"/>
+    </row>
+    <row r="44" spans="1:6" ht="21">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2887,7 +2944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="21">
+    <row r="45" spans="1:6" ht="21">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -2902,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="21">
+    <row r="46" spans="1:6" ht="21">
       <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
@@ -2917,7 +2974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="21">
+    <row r="47" spans="1:6" ht="21">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -2932,7 +2989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="21">
+    <row r="48" spans="1:6" ht="21">
       <c r="A48" s="8" t="s">
         <v>42</v>
       </c>

</xml_diff>